<commit_message>
[DSD-1088] Trimmed out the data which is exceeding 64 column size on mosip-master doc_type table.
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/doc_type.xlsx
+++ b/mosip_master/xlsx/doc_type.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="265">
   <si>
     <t xml:space="preserve">lang_code</t>
   </si>
@@ -658,9 +658,6 @@
     <t xml:space="preserve">सरकार द्वारा जारी फोटो पहचान पत्र</t>
   </si>
   <si>
-    <t xml:space="preserve">सेवा फोटो आईडी कार्ड जो एक सार्वजनिक उपक्रम द्वारा जारी किया जाता है</t>
-  </si>
-  <si>
     <t xml:space="preserve">हथियारों का लाइसेंस</t>
   </si>
   <si>
@@ -697,9 +694,6 @@
     <t xml:space="preserve">पीडीएस कार्ड</t>
   </si>
   <si>
-    <t xml:space="preserve">राज्य सरकार, सीजीएचएस, ईसीएचएस और ईएसआईसी द्वारा जारी मेडिकल कार्ड</t>
-  </si>
-  <si>
     <t xml:space="preserve">सेना का कैंटीन कार्ड</t>
   </si>
   <si>
@@ -772,9 +766,6 @@
     <t xml:space="preserve">அரசாங்கத்தால் வழங்கப்பட்ட புகைப்பட அடையாள அட்டைகள்</t>
   </si>
   <si>
-    <t xml:space="preserve">பொதுத்துறை நிறுவனத்தால் வழங்கப்படும் சேவை புகைப்பட அடையாள அட்டைகள்</t>
-  </si>
-  <si>
     <t xml:space="preserve">ஆயுத உரிமம்</t>
   </si>
   <si>
@@ -797,9 +788,6 @@
   </si>
   <si>
     <t xml:space="preserve">ரேஷன் கார்டு</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PSU ஆனது முகவரியுடன் கூடிய சேவை புகைப்பட அடையாள அட்டையை வழங்கியது</t>
   </si>
   <si>
     <t xml:space="preserve">முந்தைய 3 மாத மின் கட்டணம்</t>
@@ -966,10 +954,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E181"/>
+  <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A83" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C142" activeCellId="0" sqref="C142"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C88" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E91" activeCellId="0" sqref="E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -998,7 +986,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
@@ -1015,7 +1003,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>9</v>
       </c>
@@ -1032,7 +1020,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>11</v>
       </c>
@@ -1049,7 +1037,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>5</v>
       </c>
@@ -1066,7 +1054,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>9</v>
       </c>
@@ -1083,7 +1071,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>11</v>
       </c>
@@ -1100,7 +1088,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>5</v>
       </c>
@@ -1117,7 +1105,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>9</v>
       </c>
@@ -1134,7 +1122,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>11</v>
       </c>
@@ -1151,7 +1139,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>5</v>
       </c>
@@ -1168,7 +1156,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>9</v>
       </c>
@@ -1185,7 +1173,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>11</v>
       </c>
@@ -1202,7 +1190,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>5</v>
       </c>
@@ -1219,7 +1207,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>9</v>
       </c>
@@ -1236,7 +1224,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>11</v>
       </c>
@@ -1253,7 +1241,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>5</v>
       </c>
@@ -1270,7 +1258,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>9</v>
       </c>
@@ -1287,7 +1275,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>11</v>
       </c>
@@ -1304,7 +1292,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>5</v>
       </c>
@@ -1321,7 +1309,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>9</v>
       </c>
@@ -1338,7 +1326,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>11</v>
       </c>
@@ -1355,7 +1343,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>5</v>
       </c>
@@ -1372,7 +1360,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>5</v>
       </c>
@@ -1389,7 +1377,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>5</v>
       </c>
@@ -1406,7 +1394,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>5</v>
       </c>
@@ -1423,7 +1411,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>5</v>
       </c>
@@ -1440,7 +1428,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>5</v>
       </c>
@@ -1457,7 +1445,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>5</v>
       </c>
@@ -1474,7 +1462,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>5</v>
       </c>
@@ -1491,7 +1479,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>5</v>
       </c>
@@ -1508,7 +1496,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>5</v>
       </c>
@@ -1525,7 +1513,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>5</v>
       </c>
@@ -1542,7 +1530,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>5</v>
       </c>
@@ -1559,7 +1547,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>5</v>
       </c>
@@ -1576,7 +1564,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>5</v>
       </c>
@@ -1593,7 +1581,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>5</v>
       </c>
@@ -1610,7 +1598,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>5</v>
       </c>
@@ -1627,7 +1615,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>5</v>
       </c>
@@ -1644,7 +1632,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>5</v>
       </c>
@@ -1661,7 +1649,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>5</v>
       </c>
@@ -1678,7 +1666,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>5</v>
       </c>
@@ -1695,7 +1683,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>5</v>
       </c>
@@ -1712,7 +1700,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>5</v>
       </c>
@@ -1729,7 +1717,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>11</v>
       </c>
@@ -1746,7 +1734,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>11</v>
       </c>
@@ -1763,7 +1751,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>11</v>
       </c>
@@ -1780,7 +1768,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>11</v>
       </c>
@@ -1797,7 +1785,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>11</v>
       </c>
@@ -1814,7 +1802,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>11</v>
       </c>
@@ -1831,7 +1819,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>11</v>
       </c>
@@ -1848,7 +1836,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>11</v>
       </c>
@@ -1865,7 +1853,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>11</v>
       </c>
@@ -1882,7 +1870,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>11</v>
       </c>
@@ -1899,7 +1887,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>11</v>
       </c>
@@ -1916,7 +1904,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>11</v>
       </c>
@@ -1933,7 +1921,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>11</v>
       </c>
@@ -1950,7 +1938,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>11</v>
       </c>
@@ -1967,7 +1955,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>11</v>
       </c>
@@ -1984,7 +1972,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>11</v>
       </c>
@@ -2001,7 +1989,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>11</v>
       </c>
@@ -2018,7 +2006,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>11</v>
       </c>
@@ -2035,7 +2023,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>11</v>
       </c>
@@ -2052,7 +2040,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>11</v>
       </c>
@@ -2069,7 +2057,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>11</v>
       </c>
@@ -2086,7 +2074,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>11</v>
       </c>
@@ -2103,7 +2091,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>5</v>
       </c>
@@ -2120,7 +2108,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>11</v>
       </c>
@@ -2137,7 +2125,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>9</v>
       </c>
@@ -2154,7 +2142,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>9</v>
       </c>
@@ -2171,7 +2159,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>9</v>
       </c>
@@ -2188,7 +2176,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
         <v>9</v>
       </c>
@@ -2205,7 +2193,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
         <v>9</v>
       </c>
@@ -2222,7 +2210,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
         <v>9</v>
       </c>
@@ -2239,7 +2227,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
         <v>9</v>
       </c>
@@ -2256,7 +2244,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
         <v>9</v>
       </c>
@@ -2273,7 +2261,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
         <v>9</v>
       </c>
@@ -2290,7 +2278,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
         <v>9</v>
       </c>
@@ -2307,7 +2295,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
         <v>9</v>
       </c>
@@ -2324,7 +2312,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
         <v>9</v>
       </c>
@@ -2341,7 +2329,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
         <v>9</v>
       </c>
@@ -2358,7 +2346,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
         <v>9</v>
       </c>
@@ -2375,7 +2363,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>9</v>
       </c>
@@ -2392,7 +2380,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
         <v>9</v>
       </c>
@@ -2409,7 +2397,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
         <v>9</v>
       </c>
@@ -2426,7 +2414,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
         <v>9</v>
       </c>
@@ -2443,7 +2431,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
         <v>9</v>
       </c>
@@ -2460,7 +2448,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
         <v>9</v>
       </c>
@@ -2477,7 +2465,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>9</v>
       </c>
@@ -2494,7 +2482,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
         <v>9</v>
       </c>
@@ -2511,7 +2499,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
         <v>9</v>
       </c>
@@ -3004,7 +2992,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
         <v>153</v>
       </c>
@@ -3247,7 +3235,7 @@
         <v>193</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C134" s="0" t="s">
         <v>211</v>
@@ -3264,7 +3252,7 @@
         <v>193</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C135" s="0" t="s">
         <v>212</v>
@@ -3281,7 +3269,7 @@
         <v>193</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C136" s="0" t="s">
         <v>213</v>
@@ -3298,7 +3286,7 @@
         <v>193</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C137" s="0" t="s">
         <v>214</v>
@@ -3315,7 +3303,7 @@
         <v>193</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C138" s="0" t="s">
         <v>215</v>
@@ -3332,7 +3320,7 @@
         <v>193</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C139" s="0" t="s">
         <v>216</v>
@@ -3349,7 +3337,7 @@
         <v>193</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C140" s="0" t="s">
         <v>217</v>
@@ -3366,7 +3354,7 @@
         <v>193</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C141" s="0" t="s">
         <v>218</v>
@@ -3383,7 +3371,7 @@
         <v>193</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C142" s="0" t="s">
         <v>219</v>
@@ -3400,7 +3388,7 @@
         <v>193</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C143" s="0" t="s">
         <v>220</v>
@@ -3417,7 +3405,7 @@
         <v>193</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C144" s="0" t="s">
         <v>221</v>
@@ -3434,7 +3422,7 @@
         <v>193</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C145" s="0" t="s">
         <v>222</v>
@@ -3451,7 +3439,7 @@
         <v>193</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C146" s="0" t="s">
         <v>223</v>
@@ -3463,18 +3451,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
         <v>193</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C147" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="D147" s="5" t="s">
-        <v>224</v>
+      <c r="D147" s="0" t="s">
+        <v>225</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>8</v>
@@ -3485,81 +3473,81 @@
         <v>193</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C148" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="D148" s="5" t="s">
-        <v>225</v>
+        <v>226</v>
+      </c>
+      <c r="D148" s="0" t="s">
+        <v>227</v>
       </c>
       <c r="E148" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
         <v>193</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>94</v>
+        <v>125</v>
       </c>
       <c r="C149" s="0" t="s">
-        <v>226</v>
-      </c>
-      <c r="D149" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
+      </c>
+      <c r="D149" s="5" t="s">
+        <v>228</v>
       </c>
       <c r="E149" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>193</v>
+        <v>229</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C150" s="0" t="s">
-        <v>228</v>
+        <v>6</v>
+      </c>
+      <c r="C150" s="5" t="s">
+        <v>230</v>
       </c>
       <c r="D150" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="0" t="s">
         <v>229</v>
       </c>
-      <c r="E150" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="151" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="0" t="s">
-        <v>193</v>
-      </c>
       <c r="B151" s="1" t="s">
-        <v>125</v>
+        <v>13</v>
       </c>
       <c r="C151" s="0" t="s">
-        <v>230</v>
-      </c>
-      <c r="D151" s="5" t="s">
-        <v>230</v>
+        <v>231</v>
+      </c>
+      <c r="D151" s="0" t="s">
+        <v>232</v>
       </c>
       <c r="E151" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C152" s="5" t="s">
-        <v>232</v>
+        <v>20</v>
+      </c>
+      <c r="C152" s="0" t="s">
+        <v>233</v>
       </c>
       <c r="D152" s="0" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="E152" s="1" t="s">
         <v>8</v>
@@ -3567,16 +3555,16 @@
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C153" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D153" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E153" s="1" t="s">
         <v>8</v>
@@ -3584,16 +3572,16 @@
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="C154" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D154" s="0" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="E154" s="1" t="s">
         <v>8</v>
@@ -3601,49 +3589,49 @@
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C155" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D155" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="E155" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C156" s="0" t="s">
-        <v>239</v>
-      </c>
-      <c r="D156" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
+      </c>
+      <c r="D156" s="5" t="s">
+        <v>241</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C157" s="0" t="s">
-        <v>241</v>
-      </c>
-      <c r="D157" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="D157" s="5" t="s">
         <v>242</v>
       </c>
       <c r="E157" s="1" t="s">
@@ -3652,12 +3640,12 @@
     </row>
     <row r="158" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C158" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C158" s="5" t="s">
         <v>243</v>
       </c>
       <c r="D158" s="5" t="s">
@@ -3669,12 +3657,12 @@
     </row>
     <row r="159" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C159" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C159" s="5" t="s">
         <v>244</v>
       </c>
       <c r="D159" s="5" t="s">
@@ -3686,10 +3674,10 @@
     </row>
     <row r="160" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C160" s="5" t="s">
         <v>245</v>
@@ -3703,10 +3691,10 @@
     </row>
     <row r="161" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C161" s="5" t="s">
         <v>246</v>
@@ -3720,12 +3708,12 @@
     </row>
     <row r="162" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C162" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C162" s="0" t="s">
         <v>247</v>
       </c>
       <c r="D162" s="5" t="s">
@@ -3737,10 +3725,10 @@
     </row>
     <row r="163" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C163" s="5" t="s">
         <v>248</v>
@@ -3752,12 +3740,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C164" s="5" t="s">
         <v>249</v>
@@ -3771,12 +3759,12 @@
     </row>
     <row r="165" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C165" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C165" s="5" t="s">
         <v>250</v>
       </c>
       <c r="D165" s="5" t="s">
@@ -3788,12 +3776,12 @@
     </row>
     <row r="166" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C166" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C166" s="0" t="s">
         <v>251</v>
       </c>
       <c r="D166" s="5" t="s">
@@ -3805,10 +3793,10 @@
     </row>
     <row r="167" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C167" s="5" t="s">
         <v>252</v>
@@ -3822,10 +3810,10 @@
     </row>
     <row r="168" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C168" s="5" t="s">
         <v>253</v>
@@ -3839,12 +3827,12 @@
     </row>
     <row r="169" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C169" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C169" s="5" t="s">
         <v>254</v>
       </c>
       <c r="D169" s="5" t="s">
@@ -3856,10 +3844,10 @@
     </row>
     <row r="170" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="C170" s="5" t="s">
         <v>255</v>
@@ -3873,10 +3861,10 @@
     </row>
     <row r="171" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C171" s="5" t="s">
         <v>256</v>
@@ -3890,10 +3878,10 @@
     </row>
     <row r="172" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C172" s="5" t="s">
         <v>257</v>
@@ -3905,12 +3893,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C173" s="5" t="s">
         <v>258</v>
@@ -3924,10 +3912,10 @@
     </row>
     <row r="174" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="C174" s="5" t="s">
         <v>259</v>
@@ -3941,33 +3929,33 @@
     </row>
     <row r="175" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="C175" s="5" t="s">
         <v>260</v>
       </c>
       <c r="D175" s="5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E175" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="C176" s="5" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D176" s="5" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="E176" s="1" t="s">
         <v>8</v>
@@ -3975,89 +3963,25 @@
     </row>
     <row r="177" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>89</v>
+        <v>125</v>
       </c>
       <c r="C177" s="5" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D177" s="5" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E177" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="B178" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C178" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="D178" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="E178" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="179" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="B179" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C179" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="D179" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="E179" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="180" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="B180" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C180" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="D180" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="E180" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="181" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="B181" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C181" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="D181" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="E181" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <autoFilter ref="A1:E91"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
MOSIP-30683 Updated spanish languagle template for doc_type table. (#282)
* MOSIP-30683 Added doctype for spa language

Signed-off-by: kameshsr <kameshsr1338@gmail.com>

* MOSIP-30683 Updated spanish languagle template for doc_type table

Signed-off-by: kameshsr <kameshsr1338@gmail.com>

---------

Signed-off-by: kameshsr <kameshsr1338@gmail.com>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/doc_type.xlsx
+++ b/mosip_master/xlsx/doc_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015C37B5-C6D3-46E8-8B5E-67EFF4A8A100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7BF4D05-B22E-416D-BC71-0B78228F668B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="307">
   <si>
     <t>lang_code</t>
   </si>
@@ -918,9 +918,6 @@
     <t>Tarjeta PDS</t>
   </si>
   <si>
-    <t>Tarjeta médica emitida por el Gobierno del Estado, CGHS, ECHS y ESIC</t>
-  </si>
-  <si>
     <t>Tarjeta médica emitida por el Gobierno del Estado, CGHS, ECHS y también ESIC</t>
   </si>
   <si>
@@ -940,6 +937,18 @@
   </si>
   <si>
     <t>Tarjeta de Identidad de Referencia</t>
+  </si>
+  <si>
+    <t>Tarjeta de idintotificación de elector</t>
+  </si>
+  <si>
+    <t>Tarjeta de identificación de servicio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Factura de </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tarjeta médica emitida por el Gobierno del </t>
   </si>
 </sst>
 </file>
@@ -1324,8 +1333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F177" sqref="F177"/>
+    <sheetView tabSelected="1" topLeftCell="A190" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C200" sqref="C200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4524,7 +4533,7 @@
         <v>61</v>
       </c>
       <c r="C188" t="s">
-        <v>282</v>
+        <v>303</v>
       </c>
       <c r="D188" t="s">
         <v>282</v>
@@ -4541,7 +4550,7 @@
         <v>63</v>
       </c>
       <c r="C189" t="s">
-        <v>283</v>
+        <v>303</v>
       </c>
       <c r="D189" t="s">
         <v>283</v>
@@ -4694,7 +4703,7 @@
         <v>81</v>
       </c>
       <c r="C198" t="s">
-        <v>292</v>
+        <v>304</v>
       </c>
       <c r="D198" t="s">
         <v>292</v>
@@ -4728,7 +4737,7 @@
         <v>85</v>
       </c>
       <c r="C200" t="s">
-        <v>294</v>
+        <v>305</v>
       </c>
       <c r="D200" t="s">
         <v>294</v>
@@ -4762,10 +4771,10 @@
         <v>89</v>
       </c>
       <c r="C202" t="s">
+        <v>306</v>
+      </c>
+      <c r="D202" t="s">
         <v>296</v>
-      </c>
-      <c r="D202" t="s">
-        <v>297</v>
       </c>
       <c r="E202" t="b">
         <v>1</v>
@@ -4779,10 +4788,10 @@
         <v>92</v>
       </c>
       <c r="C203" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D203" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E203" t="b">
         <v>1</v>
@@ -4796,10 +4805,10 @@
         <v>94</v>
       </c>
       <c r="C204" t="s">
+        <v>298</v>
+      </c>
+      <c r="D204" t="s">
         <v>299</v>
-      </c>
-      <c r="D204" t="s">
-        <v>300</v>
       </c>
       <c r="E204" t="b">
         <v>1</v>
@@ -4816,7 +4825,7 @@
         <v>274</v>
       </c>
       <c r="D205" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E205" t="b">
         <v>1</v>
@@ -4830,10 +4839,10 @@
         <v>125</v>
       </c>
       <c r="C206" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D206" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E206" t="b">
         <v>1</v>
@@ -4847,10 +4856,10 @@
         <v>6</v>
       </c>
       <c r="C207" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D207" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E207" t="b">
         <v>1</v>

</xml_diff>